<commit_message>
Update v2 DvPlan annotation after review.
Signed-off-by: Bee Nee Lim <beenee.lim@dolphin.fr>
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/micro_architecture/CV32E40Pv2_FPU_register_file.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/micro_architecture/CV32E40Pv2_FPU_register_file.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\corev-v-verif\cv32e40p\docs\VerifPlans\Simulation\micro_architecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnl\Downloads\core-v-verif-cv32e40p-dev\cv32e40p\docs\VerifPlans\Simulation\micro_architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440AFCF8-EA7A-4708-A388-B2FC6BF1F232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5990F4-A5B4-4693-91DC-F12F56203F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -52,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -115,27 +126,6 @@
     <t>Forwarding paths, and write-back logic are shared for the integer and floating point operations and are not replicated.</t>
   </si>
   <si>
-    <t>Mix Integer/Floating forwarding paths:
-- Integer operation uses x_i as rD, the next floating point instruction uses f_i as a source
-- fp operation uses f_i as rD, the next integer instruction uses x_i as a source
-- Integer operation uses x_i as rD, the next float store to memory instructions uses f_i as a source
-- fp operation uses f_i as rD, the next integer store to memory instructions uses x_i as a source  
--  Integer load uses x_i as rD, the next float instruction uses f_i as a source
-- fp load uses f_i as rD, the next integer instruction uses x_i as a source</t>
-  </si>
-  <si>
-    <t>Zfinx</t>
-  </si>
-  <si>
-    <t>Zfinx uses the integer registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- fp instruction has been preceeded with an integer load using one of the fp instruction operand
-- fp instruction has been followed by an integer store using the fp destination register as a source
-- All fp instructions have been preceeded by a non-fp instruction using one of the fp instruction operand
-</t>
-  </si>
-  <si>
     <t>Test-Program Type</t>
   </si>
   <si>
@@ -146,9 +136,6 @@
   </si>
   <si>
     <t>Test-Program(s) Name(s)</t>
-  </si>
-  <si>
-    <t>corev_rand_fp_instr_data_fwd_test</t>
   </si>
   <si>
     <t>corev_rand_fp_instr_test
@@ -201,30 +188,6 @@
       <t xml:space="preserve">
 see CV32E40Pv2_test_list.xlsx</t>
     </r>
-  </si>
-  <si>
-    <t>CG: RISCV_coverage_pkg.RISCV_coverage__1.fadd_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fclass_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fcvt_s_w_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fcvt_s_wu_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fcvt_w_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fcvt_wu_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fdiv_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.feq_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fle_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.flt_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fmadd_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fmax_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fmin_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fmsub_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fmul_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fnmadd_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fnmsub_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fsgnj_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fsgnjn_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fsgnjx_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fsqrt_s_cg.cp_f*
-CG: RISCV_coverage_pkg.RISCV_coverage__1.fsub_s_cg.cp_f*</t>
   </si>
   <si>
     <t>CG: RISCV_coverage_pkg.RISCV_coverage__1.fadd_s_cg.cp_f*
@@ -274,12 +237,62 @@
   <si>
     <t>Toggle is not relevant, see revised requirement below</t>
   </si>
+  <si>
+    <t xml:space="preserve">Not applicable when PULP_ZFINX=1 because there is no f0-f31 registers. It uses x0-x31 instead. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PULP_ZFINX = 1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+see CV32E40Pv2_test_list.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <t>corev_rand_fp_instr_data_fwd_test
+cv32e40p_fp_op_fwd_instr_w_loadstore_stream</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mix Integer/Floating forwarding paths:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Non-fp instr followed by fp instr with non-fp instr dest reg same as fp instr src register (a.k.a operands)
+- fp instr followed by non-fp instr with fp instr dest reg same as non-fp instr src register (a.k.a. Operands)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">corev_rand_fp_instr_*
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -331,6 +344,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -352,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -381,14 +414,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -406,9 +433,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,14 +442,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,7 +487,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -761,30 +803,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" customWidth="1"/>
-    <col min="10" max="10" width="37.28515625" customWidth="1"/>
-    <col min="11" max="11" width="108.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="46.5546875" customWidth="1"/>
+    <col min="11" max="11" width="108.44140625" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="43.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -804,16 +846,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>7</v>
@@ -825,50 +867,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="20" t="s">
-        <v>37</v>
+      <c r="J2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="18" customFormat="1" ht="390" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23" t="s">
-        <v>30</v>
+    <row r="3" spans="1:14" s="16" customFormat="1" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>15</v>
@@ -876,59 +918,56 @@
       <c r="G3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>31</v>
+      <c r="H3" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="J3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" s="18" customFormat="1" ht="330" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="8" t="s">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
     </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>20</v>
+      <c r="E5" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>15</v>
@@ -936,56 +975,56 @@
       <c r="G5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="21" t="s">
-        <v>31</v>
+      <c r="H5" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>28</v>
+      <c r="J5" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
+    <row r="6" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>32</v>
+      <c r="H6" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="12" t="s">
-        <v>28</v>
+      <c r="J6" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>

</xml_diff>